<commit_message>
Setting data for ELC-trade connection (Inner-DK)
</commit_message>
<xml_diff>
--- a/SuppXLS/Trades/ScenTrade_ELC_TRADE.xlsx
+++ b/SuppXLS/Trades/ScenTrade_ELC_TRADE.xlsx
@@ -1,21 +1,33 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="18326"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24326"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\olex\(^_^)\ResLab\Modelling\TIMES\TIMES-DK\SuppXLS\Trades\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/2bae57ad8ea7bb4f/OneDrive/GitHub^J Inc/EnergyIsland/SuppXLS/Trades/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="140" documentId="11_747545AF201C0C8B4BADBE9E9BF30FB2354431C1" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3F39A47C-3EAC-4960-AC57-C640DCF98896}"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="45" windowWidth="16538" windowHeight="9435" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-27705" yWindow="6045" windowWidth="16875" windowHeight="10530" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="LOG" sheetId="3" r:id="rId1"/>
     <sheet name="ELC_TRADE" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -40,7 +52,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J2" authorId="1" shapeId="0" xr:uid="{00000000-0006-0000-0000-000002000000}">
+    <comment ref="N2" authorId="1" shapeId="0" xr:uid="{00000000-0006-0000-0000-000002000000}">
       <text>
         <r>
           <rPr>
@@ -53,7 +65,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="O2" authorId="1" shapeId="0" xr:uid="{00000000-0006-0000-0000-000003000000}">
+    <comment ref="S2" authorId="1" shapeId="0" xr:uid="{00000000-0006-0000-0000-000003000000}">
       <text>
         <r>
           <rPr>
@@ -71,7 +83,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="44">
   <si>
     <t>Pset_CI</t>
   </si>
@@ -124,9 +136,6 @@
     <t>EFF</t>
   </si>
   <si>
-    <t>TB_ELCC*</t>
-  </si>
-  <si>
     <t>CAP2ACT</t>
   </si>
   <si>
@@ -170,13 +179,49 @@
   </si>
   <si>
     <t>DKE and DKW instead of Allregions</t>
+  </si>
+  <si>
+    <t>DKISLBH</t>
+  </si>
+  <si>
+    <t>DKISL1</t>
+  </si>
+  <si>
+    <t>DKISL2</t>
+  </si>
+  <si>
+    <t>DKISL3</t>
+  </si>
+  <si>
+    <t>INVCOST</t>
+  </si>
+  <si>
+    <t>FIXOM</t>
+  </si>
+  <si>
+    <t>TB_ELCC_DKE_DKW_01</t>
+  </si>
+  <si>
+    <t>TB_ELCC_DKE_DKISLBH_01</t>
+  </si>
+  <si>
+    <t>START</t>
+  </si>
+  <si>
+    <t>TB_ELCC_DKW_DKISL1_01</t>
+  </si>
+  <si>
+    <t>TB_ELCC_DKW_DKISL2_01</t>
+  </si>
+  <si>
+    <t>TB_ELCC_DKW_DKISL3_01</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -251,8 +296,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -279,6 +330,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -315,7 +372,7 @@
     <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -335,18 +392,19 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="11">
     <cellStyle name="Bad 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
     <cellStyle name="Comma0 - Type3" xfId="2" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
     <cellStyle name="Fixed2 - Type2" xfId="3" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 10" xfId="4" xr:uid="{00000000-0005-0000-0000-000004000000}"/>
     <cellStyle name="Normal 2" xfId="5" xr:uid="{00000000-0005-0000-0000-000005000000}"/>
     <cellStyle name="Normal 3" xfId="6" xr:uid="{00000000-0005-0000-0000-000006000000}"/>
     <cellStyle name="Normale_Scen_UC_IND-StrucConst" xfId="7" xr:uid="{00000000-0005-0000-0000-000007000000}"/>
     <cellStyle name="Percen - Type1" xfId="8" xr:uid="{00000000-0005-0000-0000-000008000000}"/>
     <cellStyle name="Percent 2" xfId="9" xr:uid="{00000000-0005-0000-0000-000009000000}"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
     <cellStyle name="Valore valido" xfId="10" xr:uid="{00000000-0005-0000-0000-00000A000000}"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -363,7 +421,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -692,7 +750,7 @@
       <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.06640625" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="11.46484375" customWidth="1"/>
     <col min="2" max="2" width="15.59765625" customWidth="1"/>
@@ -703,19 +761,19 @@
   <sheetData>
     <row r="3" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A3" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="B3" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="B3" s="8" t="s">
+      <c r="C3" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="C3" s="8" t="s">
+      <c r="D3" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="D3" s="8" t="s">
+      <c r="E3" s="8" t="s">
         <v>28</v>
-      </c>
-      <c r="E3" s="8" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="4" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.45">
@@ -723,17 +781,17 @@
         <v>42991</v>
       </c>
       <c r="B4" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="C4" s="9" t="s">
         <v>30</v>
-      </c>
-      <c r="C4" s="9" t="s">
-        <v>31</v>
       </c>
       <c r="D4" s="9" t="str">
         <f>ADDRESS(ROW(ELC_TRADE!H3),COLUMN(ELC_TRADE!H3),4,1)&amp;","&amp;ADDRESS(ROW(ELC_TRADE!I3),COLUMN(ELC_TRADE!I3),4,1)</f>
         <v>H3,I3</v>
       </c>
       <c r="E4" s="9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
   </sheetData>
@@ -745,13 +803,13 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:Q9"/>
+  <dimension ref="A1:U33"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="J13" sqref="J13"/>
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.06640625" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="2" max="2" width="10.1328125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="8.86328125" bestFit="1" customWidth="1"/>
@@ -760,36 +818,36 @@
     <col min="6" max="6" width="11.53125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="9.6640625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="10.6640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.6640625" customWidth="1"/>
-    <col min="10" max="10" width="8.6640625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12.6640625" customWidth="1"/>
-    <col min="12" max="12" width="8.46484375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="7.53125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="8.53125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="8.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="13" width="10.6640625" customWidth="1"/>
+    <col min="14" max="14" width="8.6640625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12.6640625" customWidth="1"/>
     <col min="16" max="16" width="8.46484375" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="15" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="7.53125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="8.53125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="8.6640625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="8.46484375" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="15" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.45">
       <c r="B2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J2" s="2"/>
-      <c r="K2" s="3"/>
-      <c r="L2" s="3"/>
-      <c r="M2" s="3"/>
-      <c r="N2" s="3"/>
+      <c r="N2" s="2"/>
       <c r="O2" s="3"/>
       <c r="P2" s="3"/>
       <c r="Q2" s="3"/>
-    </row>
-    <row r="3" spans="1:17" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="R2" s="3"/>
+      <c r="S2" s="3"/>
+      <c r="T2" s="3"/>
+      <c r="U2" s="3"/>
+    </row>
+    <row r="3" spans="1:21" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B3" s="4" t="s">
         <v>9</v>
       </c>
@@ -809,37 +867,49 @@
         <v>14</v>
       </c>
       <c r="H3" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="I3" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="I3" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="J3" s="6" t="s">
+      <c r="J3" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="K3" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="L3" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="M3" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="N3" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="K3" s="6" t="s">
+      <c r="O3" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="L3" s="6" t="s">
+      <c r="P3" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="M3" s="6" t="s">
+      <c r="Q3" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="N3" s="6" t="s">
+      <c r="R3" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="O3" s="6" t="s">
+      <c r="S3" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="P3" s="6" t="s">
+      <c r="T3" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="Q3" s="6" t="s">
+      <c r="U3" s="6" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:21" x14ac:dyDescent="0.45">
       <c r="D4" t="s">
         <v>16</v>
       </c>
@@ -853,17 +923,17 @@
         <f>H4</f>
         <v>0.98</v>
       </c>
-      <c r="K4" t="s">
-        <v>17</v>
-      </c>
-      <c r="Q4" s="7"/>
-    </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.45">
+      <c r="O4" t="s">
+        <v>38</v>
+      </c>
+      <c r="U4" s="7"/>
+    </row>
+    <row r="5" spans="1:21" x14ac:dyDescent="0.45">
       <c r="C5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E5">
         <v>2010</v>
@@ -872,19 +942,20 @@
         <v>600</v>
       </c>
       <c r="I5">
-        <f t="shared" ref="I5:I9" si="0">H5</f>
+        <f t="shared" ref="I5:I10" si="0">H5</f>
         <v>600</v>
       </c>
-      <c r="K5" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.45">
+      <c r="O5" t="str">
+        <f>O4</f>
+        <v>TB_ELCC_DKE_DKW_01</v>
+      </c>
+    </row>
+    <row r="6" spans="1:21" x14ac:dyDescent="0.45">
       <c r="C6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E6">
         <v>0</v>
@@ -896,13 +967,14 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="K6" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.45">
+      <c r="O6" t="str">
+        <f t="shared" ref="O6:O9" si="1">O5</f>
+        <v>TB_ELCC_DKE_DKW_01</v>
+      </c>
+    </row>
+    <row r="7" spans="1:21" x14ac:dyDescent="0.45">
       <c r="D7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H7">
         <v>1</v>
@@ -911,13 +983,14 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="K7" t="s">
+      <c r="O7" t="str">
+        <f t="shared" si="1"/>
+        <v>TB_ELCC_DKE_DKW_01</v>
+      </c>
+    </row>
+    <row r="8" spans="1:21" x14ac:dyDescent="0.45">
+      <c r="D8" t="s">
         <v>17</v>
-      </c>
-    </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.45">
-      <c r="D8" t="s">
-        <v>18</v>
       </c>
       <c r="H8">
         <v>3.1536000000000002E-2</v>
@@ -926,13 +999,14 @@
         <f t="shared" si="0"/>
         <v>3.1536000000000002E-2</v>
       </c>
-      <c r="K8" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.45">
+      <c r="O8" t="str">
+        <f t="shared" si="1"/>
+        <v>TB_ELCC_DKE_DKW_01</v>
+      </c>
+    </row>
+    <row r="9" spans="1:21" x14ac:dyDescent="0.45">
       <c r="D9" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H9">
         <v>50</v>
@@ -941,11 +1015,418 @@
         <f t="shared" si="0"/>
         <v>50</v>
       </c>
-      <c r="K9" t="s">
+      <c r="O9" t="str">
+        <f t="shared" si="1"/>
+        <v>TB_ELCC_DKE_DKW_01</v>
+      </c>
+    </row>
+    <row r="10" spans="1:21" x14ac:dyDescent="0.45">
+      <c r="D10" t="s">
+        <v>21</v>
+      </c>
+      <c r="H10">
+        <v>50</v>
+      </c>
+      <c r="J10">
+        <f>H10</f>
+        <v>50</v>
+      </c>
+      <c r="O10" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="11" spans="1:21" x14ac:dyDescent="0.45">
+      <c r="D11" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="H11">
+        <v>1</v>
+      </c>
+      <c r="J11">
+        <f>H11</f>
+        <v>1</v>
+      </c>
+      <c r="O11" t="str">
+        <f>O10</f>
+        <v>TB_ELCC_DKE_DKISLBH_01</v>
+      </c>
+    </row>
+    <row r="12" spans="1:21" x14ac:dyDescent="0.45">
+      <c r="D12" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="H12">
+        <v>1</v>
+      </c>
+      <c r="J12">
+        <f>H12</f>
+        <v>1</v>
+      </c>
+      <c r="O12" t="str">
+        <f t="shared" ref="O12:O16" si="2">O11</f>
+        <v>TB_ELCC_DKE_DKISLBH_01</v>
+      </c>
+    </row>
+    <row r="13" spans="1:21" x14ac:dyDescent="0.45">
+      <c r="D13" t="s">
+        <v>16</v>
+      </c>
+      <c r="E13">
+        <v>2020</v>
+      </c>
+      <c r="H13">
+        <f>H4</f>
+        <v>0.98</v>
+      </c>
+      <c r="J13">
+        <f>H13</f>
+        <v>0.98</v>
+      </c>
+      <c r="O13" t="str">
+        <f t="shared" si="2"/>
+        <v>TB_ELCC_DKE_DKISLBH_01</v>
+      </c>
+    </row>
+    <row r="14" spans="1:21" x14ac:dyDescent="0.45">
+      <c r="D14" t="s">
         <v>17</v>
       </c>
+      <c r="H14">
+        <f>H8</f>
+        <v>3.1536000000000002E-2</v>
+      </c>
+      <c r="J14">
+        <f>H14</f>
+        <v>3.1536000000000002E-2</v>
+      </c>
+      <c r="O14" t="str">
+        <f t="shared" si="2"/>
+        <v>TB_ELCC_DKE_DKISLBH_01</v>
+      </c>
+    </row>
+    <row r="15" spans="1:21" x14ac:dyDescent="0.45">
+      <c r="D15" t="s">
+        <v>40</v>
+      </c>
+      <c r="H15">
+        <v>2030</v>
+      </c>
+      <c r="J15">
+        <f>H15</f>
+        <v>2030</v>
+      </c>
+      <c r="O15" t="str">
+        <f t="shared" si="2"/>
+        <v>TB_ELCC_DKE_DKISLBH_01</v>
+      </c>
+    </row>
+    <row r="16" spans="1:21" x14ac:dyDescent="0.45">
+      <c r="D16" t="s">
+        <v>21</v>
+      </c>
+      <c r="I16">
+        <v>50</v>
+      </c>
+      <c r="K16">
+        <f>I16</f>
+        <v>50</v>
+      </c>
+      <c r="O16" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="17" spans="4:15" x14ac:dyDescent="0.45">
+      <c r="D17" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="I17">
+        <v>1</v>
+      </c>
+      <c r="K17">
+        <f>I17</f>
+        <v>1</v>
+      </c>
+      <c r="O17" t="str">
+        <f>O16</f>
+        <v>TB_ELCC_DKW_DKISL1_01</v>
+      </c>
+    </row>
+    <row r="18" spans="4:15" x14ac:dyDescent="0.45">
+      <c r="D18" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="I18">
+        <v>1</v>
+      </c>
+      <c r="K18">
+        <f>I18</f>
+        <v>1</v>
+      </c>
+      <c r="O18" t="str">
+        <f t="shared" ref="O18:O21" si="3">O17</f>
+        <v>TB_ELCC_DKW_DKISL1_01</v>
+      </c>
+    </row>
+    <row r="19" spans="4:15" x14ac:dyDescent="0.45">
+      <c r="D19" t="s">
+        <v>16</v>
+      </c>
+      <c r="E19">
+        <v>2020</v>
+      </c>
+      <c r="I19">
+        <f>H4</f>
+        <v>0.98</v>
+      </c>
+      <c r="K19">
+        <f>I19</f>
+        <v>0.98</v>
+      </c>
+      <c r="O19" t="str">
+        <f t="shared" si="3"/>
+        <v>TB_ELCC_DKW_DKISL1_01</v>
+      </c>
+    </row>
+    <row r="20" spans="4:15" x14ac:dyDescent="0.45">
+      <c r="D20" t="s">
+        <v>17</v>
+      </c>
+      <c r="I20">
+        <f>I8</f>
+        <v>3.1536000000000002E-2</v>
+      </c>
+      <c r="K20">
+        <f>I20</f>
+        <v>3.1536000000000002E-2</v>
+      </c>
+      <c r="O20" t="str">
+        <f t="shared" si="3"/>
+        <v>TB_ELCC_DKW_DKISL1_01</v>
+      </c>
+    </row>
+    <row r="21" spans="4:15" x14ac:dyDescent="0.45">
+      <c r="D21" t="s">
+        <v>40</v>
+      </c>
+      <c r="I21">
+        <f>H15</f>
+        <v>2030</v>
+      </c>
+      <c r="K21">
+        <f>I21</f>
+        <v>2030</v>
+      </c>
+      <c r="O21" t="str">
+        <f t="shared" si="3"/>
+        <v>TB_ELCC_DKW_DKISL1_01</v>
+      </c>
+    </row>
+    <row r="22" spans="4:15" x14ac:dyDescent="0.45">
+      <c r="D22" t="s">
+        <v>21</v>
+      </c>
+      <c r="I22">
+        <f>I16</f>
+        <v>50</v>
+      </c>
+      <c r="L22">
+        <f>I22</f>
+        <v>50</v>
+      </c>
+      <c r="O22" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="23" spans="4:15" x14ac:dyDescent="0.45">
+      <c r="D23" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="I23">
+        <v>1</v>
+      </c>
+      <c r="L23">
+        <f>I23</f>
+        <v>1</v>
+      </c>
+      <c r="O23" t="str">
+        <f>O22</f>
+        <v>TB_ELCC_DKW_DKISL2_01</v>
+      </c>
+    </row>
+    <row r="24" spans="4:15" x14ac:dyDescent="0.45">
+      <c r="D24" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="I24">
+        <v>1</v>
+      </c>
+      <c r="L24">
+        <f>I24</f>
+        <v>1</v>
+      </c>
+      <c r="O24" t="str">
+        <f t="shared" ref="O24:O27" si="4">O23</f>
+        <v>TB_ELCC_DKW_DKISL2_01</v>
+      </c>
+    </row>
+    <row r="25" spans="4:15" x14ac:dyDescent="0.45">
+      <c r="D25" t="s">
+        <v>16</v>
+      </c>
+      <c r="E25">
+        <v>2020</v>
+      </c>
+      <c r="I25">
+        <f>I19</f>
+        <v>0.98</v>
+      </c>
+      <c r="L25">
+        <f>I25</f>
+        <v>0.98</v>
+      </c>
+      <c r="O25" t="str">
+        <f t="shared" si="4"/>
+        <v>TB_ELCC_DKW_DKISL2_01</v>
+      </c>
+    </row>
+    <row r="26" spans="4:15" x14ac:dyDescent="0.45">
+      <c r="D26" t="s">
+        <v>17</v>
+      </c>
+      <c r="I26">
+        <f t="shared" ref="I26:I27" si="5">I20</f>
+        <v>3.1536000000000002E-2</v>
+      </c>
+      <c r="L26">
+        <f t="shared" ref="L26:L28" si="6">I26</f>
+        <v>3.1536000000000002E-2</v>
+      </c>
+      <c r="O26" t="str">
+        <f t="shared" si="4"/>
+        <v>TB_ELCC_DKW_DKISL2_01</v>
+      </c>
+    </row>
+    <row r="27" spans="4:15" x14ac:dyDescent="0.45">
+      <c r="D27" t="s">
+        <v>40</v>
+      </c>
+      <c r="I27">
+        <f t="shared" si="5"/>
+        <v>2030</v>
+      </c>
+      <c r="L27">
+        <f t="shared" si="6"/>
+        <v>2030</v>
+      </c>
+      <c r="O27" t="str">
+        <f t="shared" si="4"/>
+        <v>TB_ELCC_DKW_DKISL2_01</v>
+      </c>
+    </row>
+    <row r="28" spans="4:15" x14ac:dyDescent="0.45">
+      <c r="D28" t="s">
+        <v>21</v>
+      </c>
+      <c r="I28">
+        <f>I16</f>
+        <v>50</v>
+      </c>
+      <c r="M28">
+        <f>I28</f>
+        <v>50</v>
+      </c>
+      <c r="O28" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="29" spans="4:15" x14ac:dyDescent="0.45">
+      <c r="D29" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="I29">
+        <v>1</v>
+      </c>
+      <c r="M29">
+        <f>I29</f>
+        <v>1</v>
+      </c>
+      <c r="O29" t="str">
+        <f>O28</f>
+        <v>TB_ELCC_DKW_DKISL3_01</v>
+      </c>
+    </row>
+    <row r="30" spans="4:15" x14ac:dyDescent="0.45">
+      <c r="D30" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="I30">
+        <v>1</v>
+      </c>
+      <c r="M30">
+        <f t="shared" ref="M30:M33" si="7">I30</f>
+        <v>1</v>
+      </c>
+      <c r="O30" t="str">
+        <f t="shared" ref="O30:O33" si="8">O29</f>
+        <v>TB_ELCC_DKW_DKISL3_01</v>
+      </c>
+    </row>
+    <row r="31" spans="4:15" x14ac:dyDescent="0.45">
+      <c r="D31" t="s">
+        <v>16</v>
+      </c>
+      <c r="E31">
+        <v>2020</v>
+      </c>
+      <c r="I31">
+        <f>I25</f>
+        <v>0.98</v>
+      </c>
+      <c r="M31">
+        <f t="shared" si="7"/>
+        <v>0.98</v>
+      </c>
+      <c r="O31" t="str">
+        <f t="shared" si="8"/>
+        <v>TB_ELCC_DKW_DKISL3_01</v>
+      </c>
+    </row>
+    <row r="32" spans="4:15" x14ac:dyDescent="0.45">
+      <c r="D32" t="s">
+        <v>17</v>
+      </c>
+      <c r="I32">
+        <f t="shared" ref="I32:I33" si="9">I26</f>
+        <v>3.1536000000000002E-2</v>
+      </c>
+      <c r="M32">
+        <f t="shared" si="7"/>
+        <v>3.1536000000000002E-2</v>
+      </c>
+      <c r="O32" t="str">
+        <f t="shared" si="8"/>
+        <v>TB_ELCC_DKW_DKISL3_01</v>
+      </c>
+    </row>
+    <row r="33" spans="4:15" x14ac:dyDescent="0.45">
+      <c r="D33" t="s">
+        <v>40</v>
+      </c>
+      <c r="I33">
+        <f t="shared" si="9"/>
+        <v>2030</v>
+      </c>
+      <c r="M33">
+        <f t="shared" si="7"/>
+        <v>2030</v>
+      </c>
+      <c r="O33" t="str">
+        <f t="shared" si="8"/>
+        <v>TB_ELCC_DKW_DKISL3_01</v>
+      </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="12" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Chnage prices of bornholm and ISL1
</commit_message>
<xml_diff>
--- a/SuppXLS/Trades/ScenTrade_ELC_TRADE.xlsx
+++ b/SuppXLS/Trades/ScenTrade_ELC_TRADE.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/2bae57ad8ea7bb4f/OneDrive/GitHub^J Inc/EnergyIsland/SuppXLS/Trades/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="140" documentId="11_747545AF201C0C8B4BADBE9E9BF30FB2354431C1" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3F39A47C-3EAC-4960-AC57-C640DCF98896}"/>
+  <xr:revisionPtr revIDLastSave="145" documentId="11_747545AF201C0C8B4BADBE9E9BF30FB2354431C1" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D145A848-0C70-47E9-A7FA-624C01531995}"/>
   <bookViews>
-    <workbookView xWindow="-27705" yWindow="6045" windowWidth="16875" windowHeight="10530" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="44880" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="LOG" sheetId="3" r:id="rId1"/>
@@ -806,7 +806,7 @@
   <dimension ref="A1:U33"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+      <selection activeCell="K21" sqref="K21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.06640625" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -942,7 +942,7 @@
         <v>600</v>
       </c>
       <c r="I5">
-        <f t="shared" ref="I5:I10" si="0">H5</f>
+        <f t="shared" ref="I5:I9" si="0">H5</f>
         <v>600</v>
       </c>
       <c r="O5" t="str">
@@ -1028,7 +1028,7 @@
         <v>50</v>
       </c>
       <c r="J10">
-        <f>H10</f>
+        <f t="shared" ref="J10:J15" si="2">H10</f>
         <v>50</v>
       </c>
       <c r="O10" t="s">
@@ -1040,11 +1040,11 @@
         <v>36</v>
       </c>
       <c r="H11">
-        <v>1</v>
+        <v>0.1</v>
       </c>
       <c r="J11">
-        <f>H11</f>
-        <v>1</v>
+        <f t="shared" si="2"/>
+        <v>0.1</v>
       </c>
       <c r="O11" t="str">
         <f>O10</f>
@@ -1056,14 +1056,14 @@
         <v>37</v>
       </c>
       <c r="H12">
-        <v>1</v>
+        <v>0.1</v>
       </c>
       <c r="J12">
-        <f>H12</f>
-        <v>1</v>
+        <f t="shared" si="2"/>
+        <v>0.1</v>
       </c>
       <c r="O12" t="str">
-        <f t="shared" ref="O12:O16" si="2">O11</f>
+        <f t="shared" ref="O12:O15" si="3">O11</f>
         <v>TB_ELCC_DKE_DKISLBH_01</v>
       </c>
     </row>
@@ -1079,11 +1079,11 @@
         <v>0.98</v>
       </c>
       <c r="J13">
-        <f>H13</f>
+        <f t="shared" si="2"/>
         <v>0.98</v>
       </c>
       <c r="O13" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>TB_ELCC_DKE_DKISLBH_01</v>
       </c>
     </row>
@@ -1096,11 +1096,11 @@
         <v>3.1536000000000002E-2</v>
       </c>
       <c r="J14">
-        <f>H14</f>
+        <f t="shared" si="2"/>
         <v>3.1536000000000002E-2</v>
       </c>
       <c r="O14" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>TB_ELCC_DKE_DKISLBH_01</v>
       </c>
     </row>
@@ -1112,11 +1112,11 @@
         <v>2030</v>
       </c>
       <c r="J15">
-        <f>H15</f>
+        <f t="shared" si="2"/>
         <v>2030</v>
       </c>
       <c r="O15" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>TB_ELCC_DKE_DKISLBH_01</v>
       </c>
     </row>
@@ -1128,7 +1128,7 @@
         <v>50</v>
       </c>
       <c r="K16">
-        <f>I16</f>
+        <f t="shared" ref="K16:K21" si="4">I16</f>
         <v>50</v>
       </c>
       <c r="O16" t="s">
@@ -1140,11 +1140,11 @@
         <v>36</v>
       </c>
       <c r="I17">
-        <v>1</v>
+        <v>0.1</v>
       </c>
       <c r="K17">
-        <f>I17</f>
-        <v>1</v>
+        <f t="shared" si="4"/>
+        <v>0.1</v>
       </c>
       <c r="O17" t="str">
         <f>O16</f>
@@ -1156,14 +1156,14 @@
         <v>37</v>
       </c>
       <c r="I18">
-        <v>1</v>
+        <v>0.1</v>
       </c>
       <c r="K18">
-        <f>I18</f>
-        <v>1</v>
+        <f t="shared" si="4"/>
+        <v>0.1</v>
       </c>
       <c r="O18" t="str">
-        <f t="shared" ref="O18:O21" si="3">O17</f>
+        <f t="shared" ref="O18:O21" si="5">O17</f>
         <v>TB_ELCC_DKW_DKISL1_01</v>
       </c>
     </row>
@@ -1179,11 +1179,11 @@
         <v>0.98</v>
       </c>
       <c r="K19">
-        <f>I19</f>
+        <f t="shared" si="4"/>
         <v>0.98</v>
       </c>
       <c r="O19" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>TB_ELCC_DKW_DKISL1_01</v>
       </c>
     </row>
@@ -1196,11 +1196,11 @@
         <v>3.1536000000000002E-2</v>
       </c>
       <c r="K20">
-        <f>I20</f>
+        <f t="shared" si="4"/>
         <v>3.1536000000000002E-2</v>
       </c>
       <c r="O20" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>TB_ELCC_DKW_DKISL1_01</v>
       </c>
     </row>
@@ -1213,11 +1213,11 @@
         <v>2030</v>
       </c>
       <c r="K21">
-        <f>I21</f>
+        <f t="shared" si="4"/>
         <v>2030</v>
       </c>
       <c r="O21" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>TB_ELCC_DKW_DKISL1_01</v>
       </c>
     </row>
@@ -1265,7 +1265,7 @@
         <v>1</v>
       </c>
       <c r="O24" t="str">
-        <f t="shared" ref="O24:O27" si="4">O23</f>
+        <f t="shared" ref="O24:O27" si="6">O23</f>
         <v>TB_ELCC_DKW_DKISL2_01</v>
       </c>
     </row>
@@ -1285,7 +1285,7 @@
         <v>0.98</v>
       </c>
       <c r="O25" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>TB_ELCC_DKW_DKISL2_01</v>
       </c>
     </row>
@@ -1294,15 +1294,15 @@
         <v>17</v>
       </c>
       <c r="I26">
-        <f t="shared" ref="I26:I27" si="5">I20</f>
+        <f t="shared" ref="I26:I27" si="7">I20</f>
         <v>3.1536000000000002E-2</v>
       </c>
       <c r="L26">
-        <f t="shared" ref="L26:L28" si="6">I26</f>
+        <f t="shared" ref="L26:L27" si="8">I26</f>
         <v>3.1536000000000002E-2</v>
       </c>
       <c r="O26" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>TB_ELCC_DKW_DKISL2_01</v>
       </c>
     </row>
@@ -1311,15 +1311,15 @@
         <v>40</v>
       </c>
       <c r="I27">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>2030</v>
       </c>
       <c r="L27">
+        <f t="shared" si="8"/>
+        <v>2030</v>
+      </c>
+      <c r="O27" t="str">
         <f t="shared" si="6"/>
-        <v>2030</v>
-      </c>
-      <c r="O27" t="str">
-        <f t="shared" si="4"/>
         <v>TB_ELCC_DKW_DKISL2_01</v>
       </c>
     </row>
@@ -1363,11 +1363,11 @@
         <v>1</v>
       </c>
       <c r="M30">
-        <f t="shared" ref="M30:M33" si="7">I30</f>
+        <f t="shared" ref="M30:M33" si="9">I30</f>
         <v>1</v>
       </c>
       <c r="O30" t="str">
-        <f t="shared" ref="O30:O33" si="8">O29</f>
+        <f t="shared" ref="O30:O33" si="10">O29</f>
         <v>TB_ELCC_DKW_DKISL3_01</v>
       </c>
     </row>
@@ -1383,11 +1383,11 @@
         <v>0.98</v>
       </c>
       <c r="M31">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>0.98</v>
       </c>
       <c r="O31" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>TB_ELCC_DKW_DKISL3_01</v>
       </c>
     </row>
@@ -1396,15 +1396,15 @@
         <v>17</v>
       </c>
       <c r="I32">
-        <f t="shared" ref="I32:I33" si="9">I26</f>
+        <f t="shared" ref="I32:I33" si="11">I26</f>
         <v>3.1536000000000002E-2</v>
       </c>
       <c r="M32">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>3.1536000000000002E-2</v>
       </c>
       <c r="O32" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>TB_ELCC_DKW_DKISL3_01</v>
       </c>
     </row>
@@ -1413,15 +1413,15 @@
         <v>40</v>
       </c>
       <c r="I33">
+        <f t="shared" si="11"/>
+        <v>2030</v>
+      </c>
+      <c r="M33">
         <f t="shared" si="9"/>
         <v>2030</v>
       </c>
-      <c r="M33">
-        <f t="shared" si="7"/>
-        <v>2030</v>
-      </c>
       <c r="O33" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>TB_ELCC_DKW_DKISL3_01</v>
       </c>
     </row>

</xml_diff>

<commit_message>
change in cable price
</commit_message>
<xml_diff>
--- a/SuppXLS/Trades/ScenTrade_ELC_TRADE.xlsx
+++ b/SuppXLS/Trades/ScenTrade_ELC_TRADE.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\TIMES Modeller\TIMES-TOM\SuppXLS\Trades\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E887F942-6D07-4754-B3CD-71C4E5356F11}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2992393-AE4D-493F-BCEF-D95D4158ADEC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4575" yWindow="2805" windowWidth="28800" windowHeight="15375" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="LOG" sheetId="3" r:id="rId1"/>
@@ -747,16 +747,16 @@
       <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.08984375" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.453125" customWidth="1"/>
-    <col min="2" max="2" width="15.6328125" customWidth="1"/>
-    <col min="3" max="3" width="13.7265625" customWidth="1"/>
-    <col min="4" max="4" width="19.7265625" customWidth="1"/>
-    <col min="5" max="5" width="60.1796875" customWidth="1"/>
+    <col min="1" max="1" width="11.42578125" customWidth="1"/>
+    <col min="2" max="2" width="15.5703125" customWidth="1"/>
+    <col min="3" max="3" width="13.7109375" customWidth="1"/>
+    <col min="4" max="4" width="19.7109375" customWidth="1"/>
+    <col min="5" max="5" width="60.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="8" t="s">
         <v>24</v>
       </c>
@@ -773,7 +773,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="4" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="10">
         <v>42991</v>
       </c>
@@ -802,36 +802,35 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:U29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E3" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="L10" sqref="L10"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="D30" sqref="D30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.08984375" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="10.08984375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.81640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.54296875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="5.08984375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.54296875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.6328125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.6328125" bestFit="1" customWidth="1"/>
-    <col min="9" max="13" width="10.6328125" customWidth="1"/>
-    <col min="14" max="14" width="8.6328125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="12.6328125" customWidth="1"/>
-    <col min="16" max="16" width="8.453125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="7.54296875" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="8.54296875" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="8.6328125" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="8.453125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="5.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="13" width="10.5703125" customWidth="1"/>
+    <col min="14" max="14" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12.5703125" customWidth="1"/>
+    <col min="16" max="16" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="7.5703125" bestFit="1" customWidth="1"/>
+    <col min="18" max="19" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="8.42578125" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="15" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
         <v>8</v>
       </c>
@@ -844,7 +843,7 @@
       <c r="T2" s="3"/>
       <c r="U2" s="3"/>
     </row>
-    <row r="3" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="4" t="s">
         <v>9</v>
       </c>
@@ -906,7 +905,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
       <c r="D4" t="s">
         <v>16</v>
       </c>
@@ -925,7 +924,7 @@
       </c>
       <c r="U4" s="7"/>
     </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
       <c r="C5" t="s">
         <v>20</v>
       </c>
@@ -947,7 +946,7 @@
         <v>TB_ELCC_DKE_DKW_01</v>
       </c>
     </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
       <c r="C6" t="s">
         <v>20</v>
       </c>
@@ -969,7 +968,7 @@
         <v>TB_ELCC_DKE_DKW_01</v>
       </c>
     </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
       <c r="D7" t="s">
         <v>18</v>
       </c>
@@ -985,7 +984,7 @@
         <v>TB_ELCC_DKE_DKW_01</v>
       </c>
     </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
       <c r="D8" t="s">
         <v>17</v>
       </c>
@@ -1001,7 +1000,7 @@
         <v>TB_ELCC_DKE_DKW_01</v>
       </c>
     </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
       <c r="D9" t="s">
         <v>21</v>
       </c>
@@ -1017,7 +1016,7 @@
         <v>TB_ELCC_DKE_DKW_01</v>
       </c>
     </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
       <c r="D10" t="s">
         <v>21</v>
       </c>
@@ -1032,39 +1031,39 @@
         <v>39</v>
       </c>
     </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
       <c r="D11" s="11" t="s">
         <v>36</v>
       </c>
       <c r="H11">
-        <v>1E-3</v>
+        <v>0</v>
       </c>
       <c r="J11">
         <f t="shared" si="2"/>
-        <v>1E-3</v>
+        <v>0</v>
       </c>
       <c r="O11" t="str">
         <f>O10</f>
         <v>TB_ELCC_DKE_DKISLBH_01</v>
       </c>
     </row>
-    <row r="12" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
       <c r="D12" s="11" t="s">
         <v>37</v>
       </c>
       <c r="H12">
-        <v>1E-3</v>
+        <v>0</v>
       </c>
       <c r="J12">
         <f t="shared" si="2"/>
-        <v>1E-3</v>
+        <v>0</v>
       </c>
       <c r="O12" t="str">
         <f t="shared" ref="O12:O14" si="3">O11</f>
         <v>TB_ELCC_DKE_DKISLBH_01</v>
       </c>
     </row>
-    <row r="13" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
       <c r="D13" t="s">
         <v>16</v>
       </c>
@@ -1084,7 +1083,7 @@
         <v>TB_ELCC_DKE_DKISLBH_01</v>
       </c>
     </row>
-    <row r="14" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
       <c r="D14" t="s">
         <v>17</v>
       </c>
@@ -1101,7 +1100,7 @@
         <v>TB_ELCC_DKE_DKISLBH_01</v>
       </c>
     </row>
-    <row r="15" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
       <c r="D15" t="s">
         <v>21</v>
       </c>
@@ -1116,39 +1115,39 @@
         <v>40</v>
       </c>
     </row>
-    <row r="16" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
       <c r="D16" s="11" t="s">
         <v>36</v>
       </c>
       <c r="I16">
-        <v>1E-3</v>
+        <v>0</v>
       </c>
       <c r="K16">
         <f t="shared" si="4"/>
-        <v>1E-3</v>
+        <v>0</v>
       </c>
       <c r="O16" t="str">
         <f>O15</f>
         <v>TB_ELCC_DKW_DKISL1_01</v>
       </c>
     </row>
-    <row r="17" spans="4:15" x14ac:dyDescent="0.35">
+    <row r="17" spans="4:15" x14ac:dyDescent="0.25">
       <c r="D17" s="11" t="s">
         <v>37</v>
       </c>
       <c r="I17">
-        <v>1E-3</v>
+        <v>0</v>
       </c>
       <c r="K17">
         <f t="shared" si="4"/>
-        <v>1E-3</v>
+        <v>0</v>
       </c>
       <c r="O17" t="str">
         <f t="shared" ref="O17:O19" si="5">O16</f>
         <v>TB_ELCC_DKW_DKISL1_01</v>
       </c>
     </row>
-    <row r="18" spans="4:15" x14ac:dyDescent="0.35">
+    <row r="18" spans="4:15" x14ac:dyDescent="0.25">
       <c r="D18" t="s">
         <v>16</v>
       </c>
@@ -1168,7 +1167,7 @@
         <v>TB_ELCC_DKW_DKISL1_01</v>
       </c>
     </row>
-    <row r="19" spans="4:15" x14ac:dyDescent="0.35">
+    <row r="19" spans="4:15" x14ac:dyDescent="0.25">
       <c r="D19" t="s">
         <v>17</v>
       </c>
@@ -1185,7 +1184,7 @@
         <v>TB_ELCC_DKW_DKISL1_01</v>
       </c>
     </row>
-    <row r="20" spans="4:15" x14ac:dyDescent="0.35">
+    <row r="20" spans="4:15" x14ac:dyDescent="0.25">
       <c r="D20" t="s">
         <v>21</v>
       </c>
@@ -1201,39 +1200,39 @@
         <v>41</v>
       </c>
     </row>
-    <row r="21" spans="4:15" x14ac:dyDescent="0.35">
+    <row r="21" spans="4:15" x14ac:dyDescent="0.25">
       <c r="D21" s="11" t="s">
         <v>36</v>
       </c>
       <c r="I21">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L21">
         <f>I21</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O21" t="str">
         <f>O20</f>
         <v>TB_ELCC_DKW_DKISL2_01</v>
       </c>
     </row>
-    <row r="22" spans="4:15" x14ac:dyDescent="0.35">
+    <row r="22" spans="4:15" x14ac:dyDescent="0.25">
       <c r="D22" s="11" t="s">
         <v>37</v>
       </c>
       <c r="I22">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L22">
         <f>I22</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O22" t="str">
         <f t="shared" ref="O22:O24" si="6">O21</f>
         <v>TB_ELCC_DKW_DKISL2_01</v>
       </c>
     </row>
-    <row r="23" spans="4:15" x14ac:dyDescent="0.35">
+    <row r="23" spans="4:15" x14ac:dyDescent="0.25">
       <c r="D23" t="s">
         <v>16</v>
       </c>
@@ -1253,7 +1252,7 @@
         <v>TB_ELCC_DKW_DKISL2_01</v>
       </c>
     </row>
-    <row r="24" spans="4:15" x14ac:dyDescent="0.35">
+    <row r="24" spans="4:15" x14ac:dyDescent="0.25">
       <c r="D24" t="s">
         <v>17</v>
       </c>
@@ -1270,7 +1269,7 @@
         <v>TB_ELCC_DKW_DKISL2_01</v>
       </c>
     </row>
-    <row r="25" spans="4:15" x14ac:dyDescent="0.35">
+    <row r="25" spans="4:15" x14ac:dyDescent="0.25">
       <c r="D25" t="s">
         <v>21</v>
       </c>
@@ -1286,39 +1285,39 @@
         <v>42</v>
       </c>
     </row>
-    <row r="26" spans="4:15" x14ac:dyDescent="0.35">
+    <row r="26" spans="4:15" x14ac:dyDescent="0.25">
       <c r="D26" s="11" t="s">
         <v>36</v>
       </c>
       <c r="I26">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M26">
         <f>I26</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O26" t="str">
         <f>O25</f>
         <v>TB_ELCC_DKW_DKISL3_01</v>
       </c>
     </row>
-    <row r="27" spans="4:15" x14ac:dyDescent="0.35">
+    <row r="27" spans="4:15" x14ac:dyDescent="0.25">
       <c r="D27" s="11" t="s">
         <v>37</v>
       </c>
       <c r="I27">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M27">
         <f t="shared" ref="M27:M29" si="8">I27</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O27" t="str">
         <f t="shared" ref="O27:O29" si="9">O26</f>
         <v>TB_ELCC_DKW_DKISL3_01</v>
       </c>
     </row>
-    <row r="28" spans="4:15" x14ac:dyDescent="0.35">
+    <row r="28" spans="4:15" x14ac:dyDescent="0.25">
       <c r="D28" t="s">
         <v>16</v>
       </c>
@@ -1338,7 +1337,7 @@
         <v>TB_ELCC_DKW_DKISL3_01</v>
       </c>
     </row>
-    <row r="29" spans="4:15" x14ac:dyDescent="0.35">
+    <row r="29" spans="4:15" x14ac:dyDescent="0.25">
       <c r="D29" t="s">
         <v>17</v>
       </c>

</xml_diff>

<commit_message>
Update Cable Price & Set Island Distances
</commit_message>
<xml_diff>
--- a/SuppXLS/Trades/ScenTrade_ELC_TRADE.xlsx
+++ b/SuppXLS/Trades/ScenTrade_ELC_TRADE.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\TIMES Modeller\TIMES-TOM\SuppXLS\Trades\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/2bae57ad8ea7bb4f/OneDrive/GitHub^J Inc/EnergyIsland/SuppXLS/Trades/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2992393-AE4D-493F-BCEF-D95D4158ADEC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="31" documentId="13_ncr:1_{D2992393-AE4D-493F-BCEF-D95D4158ADEC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{51A2CAF6-3585-4CF0-9BAA-51D4336B9459}"/>
   <bookViews>
-    <workbookView xWindow="4575" yWindow="2805" windowWidth="28800" windowHeight="15375" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3803" yWindow="3803" windowWidth="16875" windowHeight="10522" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="LOG" sheetId="3" r:id="rId1"/>
@@ -218,6 +218,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="168" formatCode="0.000"/>
+  </numFmts>
   <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -336,7 +339,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -355,6 +358,21 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -369,7 +387,7 @@
     <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -390,18 +408,20 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="11">
     <cellStyle name="Bad 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
     <cellStyle name="Comma0 - Type3" xfId="2" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
     <cellStyle name="Fixed2 - Type2" xfId="3" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 10" xfId="4" xr:uid="{00000000-0005-0000-0000-000004000000}"/>
     <cellStyle name="Normal 2" xfId="5" xr:uid="{00000000-0005-0000-0000-000005000000}"/>
     <cellStyle name="Normal 3" xfId="6" xr:uid="{00000000-0005-0000-0000-000006000000}"/>
     <cellStyle name="Normale_Scen_UC_IND-StrucConst" xfId="7" xr:uid="{00000000-0005-0000-0000-000007000000}"/>
     <cellStyle name="Percen - Type1" xfId="8" xr:uid="{00000000-0005-0000-0000-000008000000}"/>
     <cellStyle name="Percent 2" xfId="9" xr:uid="{00000000-0005-0000-0000-000009000000}"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
     <cellStyle name="Valore valido" xfId="10" xr:uid="{00000000-0005-0000-0000-00000A000000}"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -418,7 +438,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -747,16 +767,16 @@
       <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="11.42578125" customWidth="1"/>
-    <col min="2" max="2" width="15.5703125" customWidth="1"/>
-    <col min="3" max="3" width="13.7109375" customWidth="1"/>
-    <col min="4" max="4" width="19.7109375" customWidth="1"/>
-    <col min="5" max="5" width="60.140625" customWidth="1"/>
+    <col min="1" max="1" width="11.3984375" customWidth="1"/>
+    <col min="2" max="2" width="15.59765625" customWidth="1"/>
+    <col min="3" max="3" width="13.73046875" customWidth="1"/>
+    <col min="4" max="4" width="19.73046875" customWidth="1"/>
+    <col min="5" max="5" width="60.1328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A3" s="8" t="s">
         <v>24</v>
       </c>
@@ -773,7 +793,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="4" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A4" s="10">
         <v>42991</v>
       </c>
@@ -802,35 +822,35 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:U29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="D30" sqref="D30"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="81" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="K39" sqref="K39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="2" max="2" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="5.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="13" width="10.5703125" customWidth="1"/>
-    <col min="14" max="14" width="8.5703125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="12.5703125" customWidth="1"/>
-    <col min="16" max="16" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="7.5703125" bestFit="1" customWidth="1"/>
-    <col min="18" max="19" width="8.5703125" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.1328125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.86328125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.59765625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="5.1328125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.59765625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.59765625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.59765625" bestFit="1" customWidth="1"/>
+    <col min="9" max="13" width="10.59765625" customWidth="1"/>
+    <col min="14" max="14" width="8.59765625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12.59765625" customWidth="1"/>
+    <col min="16" max="16" width="8.3984375" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="7.59765625" bestFit="1" customWidth="1"/>
+    <col min="18" max="19" width="8.59765625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="8.3984375" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="15" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.45">
       <c r="B2" s="1" t="s">
         <v>8</v>
       </c>
@@ -843,7 +863,7 @@
       <c r="T2" s="3"/>
       <c r="U2" s="3"/>
     </row>
-    <row r="3" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:21" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B3" s="4" t="s">
         <v>9</v>
       </c>
@@ -905,7 +925,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:21" x14ac:dyDescent="0.45">
       <c r="D4" t="s">
         <v>16</v>
       </c>
@@ -924,7 +944,7 @@
       </c>
       <c r="U4" s="7"/>
     </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:21" x14ac:dyDescent="0.45">
       <c r="C5" t="s">
         <v>20</v>
       </c>
@@ -946,7 +966,7 @@
         <v>TB_ELCC_DKE_DKW_01</v>
       </c>
     </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:21" x14ac:dyDescent="0.45">
       <c r="C6" t="s">
         <v>20</v>
       </c>
@@ -968,7 +988,7 @@
         <v>TB_ELCC_DKE_DKW_01</v>
       </c>
     </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:21" x14ac:dyDescent="0.45">
       <c r="D7" t="s">
         <v>18</v>
       </c>
@@ -984,7 +1004,7 @@
         <v>TB_ELCC_DKE_DKW_01</v>
       </c>
     </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:21" x14ac:dyDescent="0.45">
       <c r="D8" t="s">
         <v>17</v>
       </c>
@@ -1000,7 +1020,7 @@
         <v>TB_ELCC_DKE_DKW_01</v>
       </c>
     </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:21" x14ac:dyDescent="0.45">
       <c r="D9" t="s">
         <v>21</v>
       </c>
@@ -1016,7 +1036,7 @@
         <v>TB_ELCC_DKE_DKW_01</v>
       </c>
     </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:21" x14ac:dyDescent="0.45">
       <c r="D10" t="s">
         <v>21</v>
       </c>
@@ -1031,39 +1051,41 @@
         <v>39</v>
       </c>
     </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:21" x14ac:dyDescent="0.45">
       <c r="D11" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="H11">
-        <v>0</v>
-      </c>
-      <c r="J11">
+      <c r="H11" s="12">
+        <v>0.22395676691729324</v>
+      </c>
+      <c r="I11" s="12"/>
+      <c r="J11" s="12">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>0.22395676691729324</v>
       </c>
       <c r="O11" t="str">
         <f>O10</f>
         <v>TB_ELCC_DKE_DKISLBH_01</v>
       </c>
     </row>
-    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:21" x14ac:dyDescent="0.45">
       <c r="D12" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="H12">
-        <v>0</v>
-      </c>
-      <c r="J12">
+      <c r="H12" s="12">
+        <v>3.947368421052632E-4</v>
+      </c>
+      <c r="I12" s="12"/>
+      <c r="J12" s="12">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>3.947368421052632E-4</v>
       </c>
       <c r="O12" t="str">
         <f t="shared" ref="O12:O14" si="3">O11</f>
         <v>TB_ELCC_DKE_DKISLBH_01</v>
       </c>
     </row>
-    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:21" x14ac:dyDescent="0.45">
       <c r="D13" t="s">
         <v>16</v>
       </c>
@@ -1083,7 +1105,7 @@
         <v>TB_ELCC_DKE_DKISLBH_01</v>
       </c>
     </row>
-    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:21" x14ac:dyDescent="0.45">
       <c r="D14" t="s">
         <v>17</v>
       </c>
@@ -1100,7 +1122,7 @@
         <v>TB_ELCC_DKE_DKISLBH_01</v>
       </c>
     </row>
-    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:21" x14ac:dyDescent="0.45">
       <c r="D15" t="s">
         <v>21</v>
       </c>
@@ -1115,39 +1137,41 @@
         <v>40</v>
       </c>
     </row>
-    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:21" x14ac:dyDescent="0.45">
       <c r="D16" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="I16">
-        <v>0</v>
-      </c>
-      <c r="K16">
+      <c r="I16" s="13">
+        <v>0.74652255639097742</v>
+      </c>
+      <c r="J16" s="12"/>
+      <c r="K16" s="12">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>0.74652255639097742</v>
       </c>
       <c r="O16" t="str">
         <f>O15</f>
         <v>TB_ELCC_DKW_DKISL1_01</v>
       </c>
     </row>
-    <row r="17" spans="4:15" x14ac:dyDescent="0.25">
+    <row r="17" spans="4:15" x14ac:dyDescent="0.45">
       <c r="D17" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="I17">
-        <v>0</v>
-      </c>
-      <c r="K17">
+      <c r="I17" s="12">
+        <v>1.3157894736842105E-3</v>
+      </c>
+      <c r="J17" s="12"/>
+      <c r="K17" s="12">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>1.3157894736842105E-3</v>
       </c>
       <c r="O17" t="str">
         <f t="shared" ref="O17:O19" si="5">O16</f>
         <v>TB_ELCC_DKW_DKISL1_01</v>
       </c>
     </row>
-    <row r="18" spans="4:15" x14ac:dyDescent="0.25">
+    <row r="18" spans="4:15" x14ac:dyDescent="0.45">
       <c r="D18" t="s">
         <v>16</v>
       </c>
@@ -1167,7 +1191,7 @@
         <v>TB_ELCC_DKW_DKISL1_01</v>
       </c>
     </row>
-    <row r="19" spans="4:15" x14ac:dyDescent="0.25">
+    <row r="19" spans="4:15" x14ac:dyDescent="0.45">
       <c r="D19" t="s">
         <v>17</v>
       </c>
@@ -1184,7 +1208,7 @@
         <v>TB_ELCC_DKW_DKISL1_01</v>
       </c>
     </row>
-    <row r="20" spans="4:15" x14ac:dyDescent="0.25">
+    <row r="20" spans="4:15" x14ac:dyDescent="0.45">
       <c r="D20" t="s">
         <v>21</v>
       </c>
@@ -1200,39 +1224,43 @@
         <v>41</v>
       </c>
     </row>
-    <row r="21" spans="4:15" x14ac:dyDescent="0.25">
+    <row r="21" spans="4:15" x14ac:dyDescent="0.45">
       <c r="D21" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="I21">
-        <v>0</v>
-      </c>
-      <c r="L21">
+      <c r="I21" s="12">
+        <v>0.97047932330827069</v>
+      </c>
+      <c r="J21" s="12"/>
+      <c r="K21" s="12"/>
+      <c r="L21" s="12">
         <f>I21</f>
-        <v>0</v>
+        <v>0.97047932330827069</v>
       </c>
       <c r="O21" t="str">
         <f>O20</f>
         <v>TB_ELCC_DKW_DKISL2_01</v>
       </c>
     </row>
-    <row r="22" spans="4:15" x14ac:dyDescent="0.25">
+    <row r="22" spans="4:15" x14ac:dyDescent="0.45">
       <c r="D22" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="I22">
-        <v>0</v>
-      </c>
-      <c r="L22">
+      <c r="I22" s="12">
+        <v>1.7105263157894738E-3</v>
+      </c>
+      <c r="J22" s="12"/>
+      <c r="K22" s="12"/>
+      <c r="L22" s="12">
         <f>I22</f>
-        <v>0</v>
+        <v>1.7105263157894738E-3</v>
       </c>
       <c r="O22" t="str">
         <f t="shared" ref="O22:O24" si="6">O21</f>
         <v>TB_ELCC_DKW_DKISL2_01</v>
       </c>
     </row>
-    <row r="23" spans="4:15" x14ac:dyDescent="0.25">
+    <row r="23" spans="4:15" x14ac:dyDescent="0.45">
       <c r="D23" t="s">
         <v>16</v>
       </c>
@@ -1252,7 +1280,7 @@
         <v>TB_ELCC_DKW_DKISL2_01</v>
       </c>
     </row>
-    <row r="24" spans="4:15" x14ac:dyDescent="0.25">
+    <row r="24" spans="4:15" x14ac:dyDescent="0.45">
       <c r="D24" t="s">
         <v>17</v>
       </c>
@@ -1269,7 +1297,7 @@
         <v>TB_ELCC_DKW_DKISL2_01</v>
       </c>
     </row>
-    <row r="25" spans="4:15" x14ac:dyDescent="0.25">
+    <row r="25" spans="4:15" x14ac:dyDescent="0.45">
       <c r="D25" t="s">
         <v>21</v>
       </c>
@@ -1285,39 +1313,45 @@
         <v>42</v>
       </c>
     </row>
-    <row r="26" spans="4:15" x14ac:dyDescent="0.25">
+    <row r="26" spans="4:15" x14ac:dyDescent="0.45">
       <c r="D26" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="I26">
-        <v>0</v>
-      </c>
-      <c r="M26">
+      <c r="I26" s="12">
+        <v>1.3437406015037594</v>
+      </c>
+      <c r="J26" s="12"/>
+      <c r="K26" s="12"/>
+      <c r="L26" s="12"/>
+      <c r="M26" s="12">
         <f>I26</f>
-        <v>0</v>
+        <v>1.3437406015037594</v>
       </c>
       <c r="O26" t="str">
         <f>O25</f>
         <v>TB_ELCC_DKW_DKISL3_01</v>
       </c>
     </row>
-    <row r="27" spans="4:15" x14ac:dyDescent="0.25">
+    <row r="27" spans="4:15" x14ac:dyDescent="0.45">
       <c r="D27" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="I27">
-        <v>0</v>
-      </c>
-      <c r="M27">
+      <c r="I27" s="12">
+        <v>2.3684210526315791E-3</v>
+      </c>
+      <c r="J27" s="12"/>
+      <c r="K27" s="12"/>
+      <c r="L27" s="12"/>
+      <c r="M27" s="12">
         <f t="shared" ref="M27:M29" si="8">I27</f>
-        <v>0</v>
+        <v>2.3684210526315791E-3</v>
       </c>
       <c r="O27" t="str">
         <f t="shared" ref="O27:O29" si="9">O26</f>
         <v>TB_ELCC_DKW_DKISL3_01</v>
       </c>
     </row>
-    <row r="28" spans="4:15" x14ac:dyDescent="0.25">
+    <row r="28" spans="4:15" x14ac:dyDescent="0.45">
       <c r="D28" t="s">
         <v>16</v>
       </c>
@@ -1337,7 +1371,7 @@
         <v>TB_ELCC_DKW_DKISL3_01</v>
       </c>
     </row>
-    <row r="29" spans="4:15" x14ac:dyDescent="0.25">
+    <row r="29" spans="4:15" x14ac:dyDescent="0.45">
       <c r="D29" t="s">
         <v>17</v>
       </c>

</xml_diff>

<commit_message>
minor changes to gain a better overview
</commit_message>
<xml_diff>
--- a/SuppXLS/Trades/ScenTrade_ELC_TRADE.xlsx
+++ b/SuppXLS/Trades/ScenTrade_ELC_TRADE.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/2bae57ad8ea7bb4f/OneDrive/GitHub^J Inc/EnergyIsland/SuppXLS/Trades/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\TIMES models\TIMES-tom\SuppXLS\Trades\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="31" documentId="13_ncr:1_{D2992393-AE4D-493F-BCEF-D95D4158ADEC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{51A2CAF6-3585-4CF0-9BAA-51D4336B9459}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A792A899-A34C-4067-9D90-50AA0915FC0A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3803" yWindow="3803" windowWidth="16875" windowHeight="10522" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="8976" yWindow="4044" windowWidth="30960" windowHeight="12204" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="LOG" sheetId="3" r:id="rId1"/>
@@ -219,7 +219,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="168" formatCode="0.000"/>
+    <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
   <fonts count="13" x14ac:knownFonts="1">
     <font>
@@ -339,7 +339,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -373,6 +373,33 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -387,7 +414,7 @@
     <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -408,20 +435,26 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="11">
     <cellStyle name="Bad 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
     <cellStyle name="Comma0 - Type3" xfId="2" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
     <cellStyle name="Fixed2 - Type2" xfId="3" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 10" xfId="4" xr:uid="{00000000-0005-0000-0000-000004000000}"/>
     <cellStyle name="Normal 2" xfId="5" xr:uid="{00000000-0005-0000-0000-000005000000}"/>
     <cellStyle name="Normal 3" xfId="6" xr:uid="{00000000-0005-0000-0000-000006000000}"/>
     <cellStyle name="Normale_Scen_UC_IND-StrucConst" xfId="7" xr:uid="{00000000-0005-0000-0000-000007000000}"/>
     <cellStyle name="Percen - Type1" xfId="8" xr:uid="{00000000-0005-0000-0000-000008000000}"/>
     <cellStyle name="Percent 2" xfId="9" xr:uid="{00000000-0005-0000-0000-000009000000}"/>
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
     <cellStyle name="Valore valido" xfId="10" xr:uid="{00000000-0005-0000-0000-00000A000000}"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -438,7 +471,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -767,16 +800,16 @@
       <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.3984375" customWidth="1"/>
-    <col min="2" max="2" width="15.59765625" customWidth="1"/>
-    <col min="3" max="3" width="13.73046875" customWidth="1"/>
-    <col min="4" max="4" width="19.73046875" customWidth="1"/>
-    <col min="5" max="5" width="60.1328125" customWidth="1"/>
+    <col min="1" max="1" width="11.44140625" customWidth="1"/>
+    <col min="2" max="2" width="15.5546875" customWidth="1"/>
+    <col min="3" max="3" width="13.77734375" customWidth="1"/>
+    <col min="4" max="4" width="19.77734375" customWidth="1"/>
+    <col min="5" max="5" width="60.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="8" t="s">
         <v>24</v>
       </c>
@@ -793,7 +826,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="4" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A4" s="10">
         <v>42991</v>
       </c>
@@ -823,34 +856,34 @@
   <dimension ref="A1:U29"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" zoomScale="81" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="K39" sqref="K39"/>
+      <selection activeCell="W21" sqref="W21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="10.1328125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.86328125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.59765625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="5.1328125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.59765625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.59765625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.59765625" bestFit="1" customWidth="1"/>
-    <col min="9" max="13" width="10.59765625" customWidth="1"/>
-    <col min="14" max="14" width="8.59765625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="12.59765625" customWidth="1"/>
-    <col min="16" max="16" width="8.3984375" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="7.59765625" bestFit="1" customWidth="1"/>
-    <col min="18" max="19" width="8.59765625" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="8.3984375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="5.109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.5546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="13" width="10.5546875" customWidth="1"/>
+    <col min="14" max="14" width="8.5546875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12.5546875" customWidth="1"/>
+    <col min="16" max="16" width="8.44140625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="7.5546875" bestFit="1" customWidth="1"/>
+    <col min="18" max="19" width="8.5546875" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="8.44140625" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="15" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.3">
       <c r="B2" s="1" t="s">
         <v>8</v>
       </c>
@@ -863,7 +896,7 @@
       <c r="T2" s="3"/>
       <c r="U2" s="3"/>
     </row>
-    <row r="3" spans="1:21" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B3" s="4" t="s">
         <v>9</v>
       </c>
@@ -925,379 +958,554 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.45">
-      <c r="D4" t="s">
+    <row r="4" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="D4" s="18" t="s">
         <v>16</v>
       </c>
-      <c r="E4">
+      <c r="E4" s="18">
         <v>2010</v>
       </c>
-      <c r="H4">
+      <c r="F4" s="18"/>
+      <c r="G4" s="18"/>
+      <c r="H4" s="18">
         <v>0.98</v>
       </c>
-      <c r="I4">
+      <c r="I4" s="18">
         <f>H4</f>
         <v>0.98</v>
       </c>
-      <c r="O4" t="s">
+      <c r="J4" s="18"/>
+      <c r="K4" s="18"/>
+      <c r="L4" s="18"/>
+      <c r="M4" s="18"/>
+      <c r="N4" s="18"/>
+      <c r="O4" s="18" t="s">
         <v>38</v>
       </c>
+      <c r="P4" s="18"/>
       <c r="U4" s="7"/>
     </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:21" x14ac:dyDescent="0.3">
       <c r="C5" t="s">
         <v>20</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D5" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="E5">
+      <c r="E5" s="14">
         <v>2010</v>
       </c>
-      <c r="H5">
+      <c r="F5" s="14"/>
+      <c r="G5" s="14"/>
+      <c r="H5" s="14">
         <v>600</v>
       </c>
-      <c r="I5">
+      <c r="I5" s="14">
         <f t="shared" ref="I5:I9" si="0">H5</f>
         <v>600</v>
       </c>
-      <c r="O5" t="str">
+      <c r="J5" s="14"/>
+      <c r="K5" s="14"/>
+      <c r="L5" s="14"/>
+      <c r="M5" s="14"/>
+      <c r="N5" s="14"/>
+      <c r="O5" s="14" t="str">
         <f>O4</f>
         <v>TB_ELCC_DKE_DKW_01</v>
       </c>
-    </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.45">
+      <c r="P5" s="14"/>
+    </row>
+    <row r="6" spans="1:21" x14ac:dyDescent="0.3">
       <c r="C6" t="s">
         <v>20</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D6" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="E6">
+      <c r="E6" s="14">
         <v>0</v>
       </c>
-      <c r="H6">
+      <c r="F6" s="14"/>
+      <c r="G6" s="14"/>
+      <c r="H6" s="14">
         <v>5</v>
       </c>
-      <c r="I6">
+      <c r="I6" s="14">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="O6" t="str">
+      <c r="J6" s="14"/>
+      <c r="K6" s="14"/>
+      <c r="L6" s="14"/>
+      <c r="M6" s="14"/>
+      <c r="N6" s="14"/>
+      <c r="O6" s="14" t="str">
         <f t="shared" ref="O6:O9" si="1">O5</f>
         <v>TB_ELCC_DKE_DKW_01</v>
       </c>
-    </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.45">
-      <c r="D7" t="s">
+      <c r="P6" s="14"/>
+    </row>
+    <row r="7" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="D7" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="H7">
+      <c r="E7" s="14"/>
+      <c r="F7" s="14"/>
+      <c r="G7" s="14"/>
+      <c r="H7" s="14">
         <v>1</v>
       </c>
-      <c r="I7">
+      <c r="I7" s="14">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="O7" t="str">
+      <c r="J7" s="14"/>
+      <c r="K7" s="14"/>
+      <c r="L7" s="14"/>
+      <c r="M7" s="14"/>
+      <c r="N7" s="14"/>
+      <c r="O7" s="14" t="str">
         <f t="shared" si="1"/>
         <v>TB_ELCC_DKE_DKW_01</v>
       </c>
-    </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.45">
-      <c r="D8" t="s">
+      <c r="P7" s="14"/>
+    </row>
+    <row r="8" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="D8" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="H8">
+      <c r="E8" s="14"/>
+      <c r="F8" s="14"/>
+      <c r="G8" s="14"/>
+      <c r="H8" s="14">
         <v>3.1536000000000002E-2</v>
       </c>
-      <c r="I8">
+      <c r="I8" s="14">
         <f t="shared" si="0"/>
         <v>3.1536000000000002E-2</v>
       </c>
-      <c r="O8" t="str">
+      <c r="J8" s="14"/>
+      <c r="K8" s="14"/>
+      <c r="L8" s="14"/>
+      <c r="M8" s="14"/>
+      <c r="N8" s="14"/>
+      <c r="O8" s="14" t="str">
         <f t="shared" si="1"/>
         <v>TB_ELCC_DKE_DKW_01</v>
       </c>
-    </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.45">
-      <c r="D9" t="s">
+      <c r="P8" s="14"/>
+    </row>
+    <row r="9" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="D9" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="H9">
+      <c r="E9" s="17"/>
+      <c r="F9" s="17"/>
+      <c r="G9" s="17"/>
+      <c r="H9" s="17">
         <v>50</v>
       </c>
-      <c r="I9">
+      <c r="I9" s="17">
         <f t="shared" si="0"/>
         <v>50</v>
       </c>
-      <c r="O9" t="str">
+      <c r="J9" s="17"/>
+      <c r="K9" s="17"/>
+      <c r="L9" s="17"/>
+      <c r="M9" s="17"/>
+      <c r="N9" s="17"/>
+      <c r="O9" s="17" t="str">
         <f t="shared" si="1"/>
         <v>TB_ELCC_DKE_DKW_01</v>
       </c>
-    </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.45">
-      <c r="D10" t="s">
+      <c r="P9" s="17"/>
+    </row>
+    <row r="10" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="D10" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="H10">
+      <c r="E10" s="14"/>
+      <c r="F10" s="14"/>
+      <c r="G10" s="14"/>
+      <c r="H10" s="14">
         <v>50</v>
       </c>
-      <c r="J10">
+      <c r="I10" s="14"/>
+      <c r="J10" s="14">
         <f t="shared" ref="J10:J14" si="2">H10</f>
         <v>50</v>
       </c>
-      <c r="O10" t="s">
+      <c r="K10" s="14"/>
+      <c r="L10" s="14"/>
+      <c r="M10" s="14"/>
+      <c r="N10" s="14"/>
+      <c r="O10" s="14" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.45">
-      <c r="D11" s="11" t="s">
+      <c r="P10" s="14"/>
+    </row>
+    <row r="11" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="D11" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="H11" s="12">
+      <c r="E11" s="14"/>
+      <c r="F11" s="14"/>
+      <c r="G11" s="14"/>
+      <c r="H11" s="16">
         <v>0.22395676691729324</v>
       </c>
-      <c r="I11" s="12"/>
-      <c r="J11" s="12">
+      <c r="I11" s="16"/>
+      <c r="J11" s="16">
         <f t="shared" si="2"/>
         <v>0.22395676691729324</v>
       </c>
-      <c r="O11" t="str">
+      <c r="K11" s="14"/>
+      <c r="L11" s="14"/>
+      <c r="M11" s="14"/>
+      <c r="N11" s="14"/>
+      <c r="O11" s="14" t="str">
         <f>O10</f>
         <v>TB_ELCC_DKE_DKISLBH_01</v>
       </c>
-    </row>
-    <row r="12" spans="1:21" x14ac:dyDescent="0.45">
-      <c r="D12" s="11" t="s">
+      <c r="P11" s="14"/>
+    </row>
+    <row r="12" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="D12" s="15" t="s">
         <v>37</v>
       </c>
-      <c r="H12" s="12">
+      <c r="E12" s="14"/>
+      <c r="F12" s="14"/>
+      <c r="G12" s="14"/>
+      <c r="H12" s="16">
         <v>3.947368421052632E-4</v>
       </c>
-      <c r="I12" s="12"/>
-      <c r="J12" s="12">
+      <c r="I12" s="16"/>
+      <c r="J12" s="16">
         <f t="shared" si="2"/>
         <v>3.947368421052632E-4</v>
       </c>
-      <c r="O12" t="str">
+      <c r="K12" s="14"/>
+      <c r="L12" s="14"/>
+      <c r="M12" s="14"/>
+      <c r="N12" s="14"/>
+      <c r="O12" s="14" t="str">
         <f t="shared" ref="O12:O14" si="3">O11</f>
         <v>TB_ELCC_DKE_DKISLBH_01</v>
       </c>
-    </row>
-    <row r="13" spans="1:21" x14ac:dyDescent="0.45">
-      <c r="D13" t="s">
+      <c r="P12" s="14"/>
+    </row>
+    <row r="13" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="D13" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="E13">
-        <v>2020</v>
-      </c>
-      <c r="H13">
+      <c r="E13" s="14">
+        <v>2030</v>
+      </c>
+      <c r="F13" s="14"/>
+      <c r="G13" s="14"/>
+      <c r="H13" s="14">
         <f>H4</f>
         <v>0.98</v>
       </c>
-      <c r="J13">
+      <c r="I13" s="14"/>
+      <c r="J13" s="14">
         <f t="shared" si="2"/>
         <v>0.98</v>
       </c>
-      <c r="O13" t="str">
+      <c r="K13" s="14"/>
+      <c r="L13" s="14"/>
+      <c r="M13" s="14"/>
+      <c r="N13" s="14"/>
+      <c r="O13" s="14" t="str">
         <f t="shared" si="3"/>
         <v>TB_ELCC_DKE_DKISLBH_01</v>
       </c>
-    </row>
-    <row r="14" spans="1:21" x14ac:dyDescent="0.45">
-      <c r="D14" t="s">
+      <c r="P13" s="14"/>
+    </row>
+    <row r="14" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="D14" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="H14">
+      <c r="E14" s="17"/>
+      <c r="F14" s="17"/>
+      <c r="G14" s="17"/>
+      <c r="H14" s="17">
         <f>H8</f>
         <v>3.1536000000000002E-2</v>
       </c>
-      <c r="J14">
+      <c r="I14" s="17"/>
+      <c r="J14" s="17">
         <f t="shared" si="2"/>
         <v>3.1536000000000002E-2</v>
       </c>
-      <c r="O14" t="str">
+      <c r="K14" s="17"/>
+      <c r="L14" s="17"/>
+      <c r="M14" s="17"/>
+      <c r="N14" s="17"/>
+      <c r="O14" s="17" t="str">
         <f t="shared" si="3"/>
         <v>TB_ELCC_DKE_DKISLBH_01</v>
       </c>
-    </row>
-    <row r="15" spans="1:21" x14ac:dyDescent="0.45">
-      <c r="D15" t="s">
+      <c r="P14" s="17"/>
+    </row>
+    <row r="15" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="D15" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="I15">
+      <c r="E15" s="14"/>
+      <c r="F15" s="14"/>
+      <c r="G15" s="14"/>
+      <c r="H15" s="14"/>
+      <c r="I15" s="14">
         <v>50</v>
       </c>
-      <c r="K15">
+      <c r="J15" s="14"/>
+      <c r="K15" s="14">
         <f t="shared" ref="K15:K19" si="4">I15</f>
         <v>50</v>
       </c>
-      <c r="O15" t="s">
+      <c r="L15" s="14"/>
+      <c r="M15" s="14"/>
+      <c r="N15" s="14"/>
+      <c r="O15" s="14" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="16" spans="1:21" x14ac:dyDescent="0.45">
-      <c r="D16" s="11" t="s">
+      <c r="P15" s="14"/>
+    </row>
+    <row r="16" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="D16" s="15" t="s">
         <v>36</v>
       </c>
+      <c r="E16" s="14"/>
+      <c r="F16" s="14"/>
+      <c r="G16" s="14"/>
+      <c r="H16" s="14"/>
       <c r="I16" s="13">
         <v>0.74652255639097742</v>
       </c>
-      <c r="J16" s="12"/>
-      <c r="K16" s="12">
+      <c r="J16" s="16"/>
+      <c r="K16" s="16">
         <f t="shared" si="4"/>
         <v>0.74652255639097742</v>
       </c>
-      <c r="O16" t="str">
+      <c r="L16" s="14"/>
+      <c r="M16" s="14"/>
+      <c r="N16" s="14"/>
+      <c r="O16" s="14" t="str">
         <f>O15</f>
         <v>TB_ELCC_DKW_DKISL1_01</v>
       </c>
-    </row>
-    <row r="17" spans="4:15" x14ac:dyDescent="0.45">
-      <c r="D17" s="11" t="s">
+      <c r="P16" s="14"/>
+    </row>
+    <row r="17" spans="4:16" x14ac:dyDescent="0.3">
+      <c r="D17" s="15" t="s">
         <v>37</v>
       </c>
-      <c r="I17" s="12">
+      <c r="E17" s="14"/>
+      <c r="F17" s="14"/>
+      <c r="G17" s="14"/>
+      <c r="H17" s="14"/>
+      <c r="I17" s="16">
         <v>1.3157894736842105E-3</v>
       </c>
-      <c r="J17" s="12"/>
-      <c r="K17" s="12">
+      <c r="J17" s="16"/>
+      <c r="K17" s="16">
         <f t="shared" si="4"/>
         <v>1.3157894736842105E-3</v>
       </c>
-      <c r="O17" t="str">
+      <c r="L17" s="14"/>
+      <c r="M17" s="14"/>
+      <c r="N17" s="14"/>
+      <c r="O17" s="14" t="str">
         <f t="shared" ref="O17:O19" si="5">O16</f>
         <v>TB_ELCC_DKW_DKISL1_01</v>
       </c>
-    </row>
-    <row r="18" spans="4:15" x14ac:dyDescent="0.45">
-      <c r="D18" t="s">
+      <c r="P17" s="14"/>
+    </row>
+    <row r="18" spans="4:16" x14ac:dyDescent="0.3">
+      <c r="D18" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="E18">
-        <v>2020</v>
-      </c>
-      <c r="I18">
+      <c r="E18" s="14">
+        <v>2030</v>
+      </c>
+      <c r="F18" s="14"/>
+      <c r="G18" s="14"/>
+      <c r="H18" s="14"/>
+      <c r="I18" s="14">
         <f>H4</f>
         <v>0.98</v>
       </c>
-      <c r="K18">
+      <c r="J18" s="14"/>
+      <c r="K18" s="14">
         <f t="shared" si="4"/>
         <v>0.98</v>
       </c>
-      <c r="O18" t="str">
+      <c r="L18" s="14"/>
+      <c r="M18" s="14"/>
+      <c r="N18" s="14"/>
+      <c r="O18" s="14" t="str">
         <f t="shared" si="5"/>
         <v>TB_ELCC_DKW_DKISL1_01</v>
       </c>
-    </row>
-    <row r="19" spans="4:15" x14ac:dyDescent="0.45">
-      <c r="D19" t="s">
+      <c r="P18" s="14"/>
+    </row>
+    <row r="19" spans="4:16" x14ac:dyDescent="0.3">
+      <c r="D19" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="I19">
+      <c r="E19" s="17"/>
+      <c r="F19" s="17"/>
+      <c r="G19" s="17"/>
+      <c r="H19" s="17"/>
+      <c r="I19" s="17">
         <f>I8</f>
         <v>3.1536000000000002E-2</v>
       </c>
-      <c r="K19">
+      <c r="J19" s="17"/>
+      <c r="K19" s="17">
         <f t="shared" si="4"/>
         <v>3.1536000000000002E-2</v>
       </c>
-      <c r="O19" t="str">
+      <c r="L19" s="17"/>
+      <c r="M19" s="17"/>
+      <c r="N19" s="17"/>
+      <c r="O19" s="17" t="str">
         <f t="shared" si="5"/>
         <v>TB_ELCC_DKW_DKISL1_01</v>
       </c>
-    </row>
-    <row r="20" spans="4:15" x14ac:dyDescent="0.45">
-      <c r="D20" t="s">
+      <c r="P19" s="17"/>
+    </row>
+    <row r="20" spans="4:16" x14ac:dyDescent="0.3">
+      <c r="D20" s="19" t="s">
         <v>21</v>
       </c>
-      <c r="I20">
+      <c r="E20" s="19"/>
+      <c r="F20" s="19"/>
+      <c r="G20" s="19"/>
+      <c r="H20" s="19"/>
+      <c r="I20" s="19">
         <f>I15</f>
         <v>50</v>
       </c>
-      <c r="L20">
+      <c r="J20" s="19"/>
+      <c r="K20" s="19"/>
+      <c r="L20" s="19">
         <f>I20</f>
         <v>50</v>
       </c>
-      <c r="O20" t="s">
+      <c r="M20" s="19"/>
+      <c r="N20" s="19"/>
+      <c r="O20" s="19" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="21" spans="4:15" x14ac:dyDescent="0.45">
-      <c r="D21" s="11" t="s">
+      <c r="P20" s="19"/>
+    </row>
+    <row r="21" spans="4:16" x14ac:dyDescent="0.3">
+      <c r="D21" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="I21" s="12">
+      <c r="E21" s="14"/>
+      <c r="F21" s="14"/>
+      <c r="G21" s="14"/>
+      <c r="H21" s="14"/>
+      <c r="I21" s="16">
         <v>0.97047932330827069</v>
       </c>
-      <c r="J21" s="12"/>
-      <c r="K21" s="12"/>
-      <c r="L21" s="12">
+      <c r="J21" s="16"/>
+      <c r="K21" s="16"/>
+      <c r="L21" s="16">
         <f>I21</f>
         <v>0.97047932330827069</v>
       </c>
-      <c r="O21" t="str">
+      <c r="M21" s="14"/>
+      <c r="N21" s="14"/>
+      <c r="O21" s="14" t="str">
         <f>O20</f>
         <v>TB_ELCC_DKW_DKISL2_01</v>
       </c>
-    </row>
-    <row r="22" spans="4:15" x14ac:dyDescent="0.45">
-      <c r="D22" s="11" t="s">
+      <c r="P21" s="14"/>
+    </row>
+    <row r="22" spans="4:16" x14ac:dyDescent="0.3">
+      <c r="D22" s="15" t="s">
         <v>37</v>
       </c>
-      <c r="I22" s="12">
+      <c r="E22" s="14"/>
+      <c r="F22" s="14"/>
+      <c r="G22" s="14"/>
+      <c r="H22" s="14"/>
+      <c r="I22" s="16">
         <v>1.7105263157894738E-3</v>
       </c>
-      <c r="J22" s="12"/>
-      <c r="K22" s="12"/>
-      <c r="L22" s="12">
+      <c r="J22" s="16"/>
+      <c r="K22" s="16"/>
+      <c r="L22" s="16">
         <f>I22</f>
         <v>1.7105263157894738E-3</v>
       </c>
-      <c r="O22" t="str">
+      <c r="M22" s="14"/>
+      <c r="N22" s="14"/>
+      <c r="O22" s="14" t="str">
         <f t="shared" ref="O22:O24" si="6">O21</f>
         <v>TB_ELCC_DKW_DKISL2_01</v>
       </c>
-    </row>
-    <row r="23" spans="4:15" x14ac:dyDescent="0.45">
-      <c r="D23" t="s">
+      <c r="P22" s="14"/>
+    </row>
+    <row r="23" spans="4:16" x14ac:dyDescent="0.3">
+      <c r="D23" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="E23">
-        <v>2020</v>
-      </c>
-      <c r="I23">
+      <c r="E23" s="14">
+        <v>2030</v>
+      </c>
+      <c r="F23" s="14"/>
+      <c r="G23" s="14"/>
+      <c r="H23" s="14"/>
+      <c r="I23" s="14">
         <f>I18</f>
         <v>0.98</v>
       </c>
-      <c r="L23">
+      <c r="J23" s="14"/>
+      <c r="K23" s="14"/>
+      <c r="L23" s="14">
         <f>I23</f>
         <v>0.98</v>
       </c>
-      <c r="O23" t="str">
+      <c r="M23" s="14"/>
+      <c r="N23" s="14"/>
+      <c r="O23" s="14" t="str">
         <f t="shared" si="6"/>
         <v>TB_ELCC_DKW_DKISL2_01</v>
       </c>
-    </row>
-    <row r="24" spans="4:15" x14ac:dyDescent="0.45">
-      <c r="D24" t="s">
+      <c r="P23" s="14"/>
+    </row>
+    <row r="24" spans="4:16" x14ac:dyDescent="0.3">
+      <c r="D24" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="I24">
+      <c r="E24" s="17"/>
+      <c r="F24" s="17"/>
+      <c r="G24" s="17"/>
+      <c r="H24" s="17"/>
+      <c r="I24" s="17">
         <f>I19</f>
         <v>3.1536000000000002E-2</v>
       </c>
-      <c r="L24">
+      <c r="J24" s="17"/>
+      <c r="K24" s="17"/>
+      <c r="L24" s="17">
         <f t="shared" ref="L24" si="7">I24</f>
         <v>3.1536000000000002E-2</v>
       </c>
-      <c r="O24" t="str">
+      <c r="M24" s="17"/>
+      <c r="N24" s="17"/>
+      <c r="O24" s="17" t="str">
         <f t="shared" si="6"/>
         <v>TB_ELCC_DKW_DKISL2_01</v>
       </c>
-    </row>
-    <row r="25" spans="4:15" x14ac:dyDescent="0.45">
+      <c r="P24" s="17"/>
+    </row>
+    <row r="25" spans="4:16" x14ac:dyDescent="0.3">
       <c r="D25" t="s">
         <v>21</v>
       </c>
@@ -1313,7 +1521,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="26" spans="4:15" x14ac:dyDescent="0.45">
+    <row r="26" spans="4:16" x14ac:dyDescent="0.3">
       <c r="D26" s="11" t="s">
         <v>36</v>
       </c>
@@ -1332,7 +1540,7 @@
         <v>TB_ELCC_DKW_DKISL3_01</v>
       </c>
     </row>
-    <row r="27" spans="4:15" x14ac:dyDescent="0.45">
+    <row r="27" spans="4:16" x14ac:dyDescent="0.3">
       <c r="D27" s="11" t="s">
         <v>37</v>
       </c>
@@ -1351,12 +1559,12 @@
         <v>TB_ELCC_DKW_DKISL3_01</v>
       </c>
     </row>
-    <row r="28" spans="4:15" x14ac:dyDescent="0.45">
+    <row r="28" spans="4:16" x14ac:dyDescent="0.3">
       <c r="D28" t="s">
         <v>16</v>
       </c>
       <c r="E28">
-        <v>2020</v>
+        <v>2030</v>
       </c>
       <c r="I28">
         <f>I23</f>
@@ -1371,7 +1579,7 @@
         <v>TB_ELCC_DKW_DKISL3_01</v>
       </c>
     </row>
-    <row r="29" spans="4:15" x14ac:dyDescent="0.45">
+    <row r="29" spans="4:16" x14ac:dyDescent="0.3">
       <c r="D29" t="s">
         <v>17</v>
       </c>

</xml_diff>